<commit_message>
feat: change way to styling xlsx file
</commit_message>
<xml_diff>
--- a/internal/logconv/testdata/log.xlsx
+++ b/internal/logconv/testdata/log.xlsx
@@ -118,145 +118,145 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF89C923"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF89C923"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF2D00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF2D00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
-      <alignment/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
-      <alignment/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color rgb="FF89C923"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color rgb="FFDDA100"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color rgb="FFFF2D00"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FF89C923"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFDDA100"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFF2D00"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <diagonal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
@@ -528,19 +528,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" style="2" width="20"/>
-    <col customWidth="true" max="3" min="3" style="3" width="15"/>
-    <col customWidth="true" max="4" min="4" width="30"/>
+    <col customWidth="true" max="1" min="1" width="20"/>
+    <col customWidth="true" max="3" min="3" width="15"/>
+    <col customWidth="true" max="5" min="4" width="30"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -559,169 +559,135 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" s="1" customFormat="true">
       <c r="A2" s="2">
         <v>44198.62783564815</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>123.456</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2">
+    <row r="3" s="5" customFormat="true">
+      <c r="A3" s="6">
         <v>44198.62783564815</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="8">
         <v>12.345</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" s="1" customFormat="true">
       <c r="A4" s="2">
         <v>44198.627847222226</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>234.567</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" s="1" customFormat="true">
       <c r="A5" s="2">
         <v>44198.627847222226</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>54.321</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" s="1" customFormat="true">
       <c r="A6" s="2">
         <v>44198.627858796295</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>345.678</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2">
+    <row r="7" s="9" customFormat="true">
+      <c r="A7" s="10">
         <v>44198.62787037037</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="12">
         <v>1.234</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2">
+    <row r="8" s="13" customFormat="true">
+      <c r="A8" s="14">
         <v>44198.62788194444</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="16">
         <v>2.345</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="13" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$H$1"/>
-  <conditionalFormatting sqref="B:B">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"HEALTHY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"DEGRADE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"FAILURE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"ABORTED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A:H">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>=$B1="HEALTHY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>=$B1="DEGRADE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>=$B1="FAILURE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>=$B1="UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>=$B1="ABORTED"</formula>
-    </cfRule>
-  </conditionalFormatting>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: change timezone for log.xlsx to local of the server
</commit_message>
<xml_diff>
--- a/internal/logconv/testdata/log.xlsx
+++ b/internal/logconv/testdata/log.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>time</t>
+    <t>time (UTC)</t>
   </si>
   <si>
     <t>status</t>
@@ -99,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss&quot;Z&quot;"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="#,##0.000 &quot;ms&quot;"/>
   </numFmts>
   <fonts count="1">

</xml_diff>